<commit_message>
Cambios en el check y subtotal
</commit_message>
<xml_diff>
--- a/database/seeds/Catalogos/Licencias.xlsx
+++ b/database/seeds/Catalogos/Licencias.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$A$924</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$A$925</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Vehículo</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Ninguna</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -425,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B924"/>
+  <dimension ref="A1:B925"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,11 +443,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,7 +455,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -457,12 +463,17 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
@@ -488,7 +499,7 @@
       <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -500,7 +511,7 @@
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -716,13 +727,13 @@
       <c r="A88" s="1"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="3"/>
+      <c r="A89" s="1"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
+      <c r="A91" s="3"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
@@ -740,7 +751,7 @@
       <c r="A96" s="1"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3"/>
+      <c r="A97" s="1"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
@@ -752,7 +763,7 @@
       <c r="A100" s="3"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
+      <c r="A101" s="3"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
@@ -836,16 +847,16 @@
       <c r="A128" s="1"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="3"/>
+      <c r="A129" s="1"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="4"/>
+      <c r="A130" s="3"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
+      <c r="A132" s="4"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
@@ -947,7 +958,7 @@
       <c r="A165" s="1"/>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="3"/>
+      <c r="A166" s="1"/>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
@@ -956,16 +967,16 @@
       <c r="A168" s="3"/>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="1"/>
+      <c r="A169" s="3"/>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="3"/>
+      <c r="A171" s="1"/>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="1"/>
+      <c r="A172" s="3"/>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
@@ -1304,7 +1315,7 @@
       <c r="A284" s="1"/>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="3"/>
+      <c r="A285" s="1"/>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="3"/>
@@ -1313,7 +1324,7 @@
       <c r="A287" s="3"/>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="1"/>
+      <c r="A288" s="3"/>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="1"/>
@@ -1334,10 +1345,10 @@
       <c r="A294" s="1"/>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A295" s="4"/>
+      <c r="A295" s="1"/>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="1"/>
+      <c r="A296" s="4"/>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A297" s="1"/>
@@ -1349,7 +1360,7 @@
       <c r="A299" s="1"/>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A300" s="3"/>
+      <c r="A300" s="1"/>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A301" s="3"/>
@@ -1385,7 +1396,7 @@
       <c r="A311" s="3"/>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="1"/>
+      <c r="A312" s="3"/>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A313" s="1"/>
@@ -1556,7 +1567,7 @@
       <c r="A368" s="1"/>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="5"/>
+      <c r="A369" s="1"/>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="5"/>
@@ -1571,16 +1582,16 @@
       <c r="A373" s="5"/>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="6"/>
+      <c r="A374" s="5"/>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="5"/>
+      <c r="A375" s="6"/>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="5"/>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="6"/>
+      <c r="A377" s="5"/>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="6"/>
@@ -1592,19 +1603,19 @@
       <c r="A380" s="6"/>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="5"/>
+      <c r="A381" s="6"/>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="5"/>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="6"/>
+      <c r="A383" s="5"/>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" s="6"/>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385" s="5"/>
+      <c r="A385" s="6"/>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" s="5"/>
@@ -1613,13 +1624,13 @@
       <c r="A387" s="5"/>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="6"/>
+      <c r="A388" s="5"/>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A389" s="6"/>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="5"/>
+      <c r="A390" s="6"/>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A391" s="5"/>
@@ -1631,7 +1642,7 @@
       <c r="A393" s="5"/>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="6"/>
+      <c r="A394" s="5"/>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A395" s="6"/>
@@ -1658,7 +1669,7 @@
       <c r="A402" s="6"/>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="5"/>
+      <c r="A403" s="6"/>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A404" s="5"/>
@@ -1679,7 +1690,7 @@
       <c r="A409" s="5"/>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="6"/>
+      <c r="A410" s="5"/>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A411" s="6"/>
@@ -1688,10 +1699,10 @@
       <c r="A412" s="6"/>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="5"/>
+      <c r="A413" s="6"/>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="6"/>
+      <c r="A414" s="5"/>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="6"/>
@@ -1706,7 +1717,7 @@
       <c r="A418" s="6"/>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="5"/>
+      <c r="A419" s="6"/>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" s="5"/>
@@ -1718,7 +1729,7 @@
       <c r="A422" s="5"/>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="6"/>
+      <c r="A423" s="5"/>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A424" s="6"/>
@@ -1727,7 +1738,7 @@
       <c r="A425" s="6"/>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="5"/>
+      <c r="A426" s="6"/>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A427" s="5"/>
@@ -1757,7 +1768,7 @@
       <c r="A435" s="5"/>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="6"/>
+      <c r="A436" s="5"/>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A437" s="6"/>
@@ -1787,13 +1798,13 @@
       <c r="A445" s="6"/>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="5"/>
+      <c r="A446" s="6"/>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" s="5"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="6"/>
+      <c r="A448" s="5"/>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A449" s="6"/>
@@ -1805,7 +1816,7 @@
       <c r="A451" s="6"/>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="5"/>
+      <c r="A452" s="6"/>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A453" s="5"/>
@@ -1820,16 +1831,16 @@
       <c r="A456" s="5"/>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="7"/>
+      <c r="A457" s="5"/>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="5"/>
+      <c r="A458" s="7"/>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A459" s="5"/>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="6"/>
+      <c r="A460" s="5"/>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" s="6"/>
@@ -1838,7 +1849,7 @@
       <c r="A462" s="6"/>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="5"/>
+      <c r="A463" s="6"/>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A464" s="5"/>
@@ -1847,25 +1858,25 @@
       <c r="A465" s="5"/>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="6"/>
+      <c r="A466" s="5"/>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="5"/>
+      <c r="A467" s="6"/>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A468" s="6"/>
+      <c r="A468" s="5"/>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A469" s="6"/>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="5"/>
+      <c r="A470" s="6"/>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" s="5"/>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" s="6"/>
+      <c r="A472" s="5"/>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A473" s="6"/>
@@ -1874,13 +1885,13 @@
       <c r="A474" s="6"/>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" s="7"/>
+      <c r="A475" s="6"/>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A476" s="7"/>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A477" s="5"/>
+      <c r="A477" s="7"/>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A478" s="5"/>
@@ -1913,13 +1924,13 @@
       <c r="A487" s="5"/>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488" s="6"/>
+      <c r="A488" s="5"/>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A489" s="6"/>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490" s="5"/>
+      <c r="A490" s="6"/>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A491" s="5"/>
@@ -1955,7 +1966,7 @@
       <c r="A501" s="5"/>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A502" s="6"/>
+      <c r="A502" s="5"/>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A503" s="6"/>
@@ -1964,7 +1975,7 @@
       <c r="A504" s="6"/>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A505" s="5"/>
+      <c r="A505" s="6"/>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A506" s="5"/>
@@ -2000,10 +2011,10 @@
       <c r="A516" s="5"/>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A517" s="7"/>
+      <c r="A517" s="5"/>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A518" s="5"/>
+      <c r="A518" s="7"/>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" s="5"/>
@@ -2012,13 +2023,13 @@
       <c r="A520" s="5"/>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A521" s="7"/>
+      <c r="A521" s="5"/>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A522" s="6"/>
+      <c r="A522" s="7"/>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A523" s="5"/>
+      <c r="A523" s="6"/>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A524" s="5"/>
@@ -2033,10 +2044,10 @@
       <c r="A527" s="5"/>
     </row>
     <row r="528" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A528" s="7"/>
+      <c r="A528" s="5"/>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A529" s="5"/>
+      <c r="A529" s="7"/>
     </row>
     <row r="530" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A530" s="5"/>
@@ -2057,19 +2068,19 @@
       <c r="A535" s="5"/>
     </row>
     <row r="536" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A536" s="6"/>
+      <c r="A536" s="5"/>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A537" s="6"/>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A538" s="5"/>
+      <c r="A538" s="6"/>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A539" s="5"/>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A540" s="6"/>
+      <c r="A540" s="5"/>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A541" s="6"/>
@@ -2084,7 +2095,7 @@
       <c r="A544" s="6"/>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A545" s="5"/>
+      <c r="A545" s="6"/>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A546" s="5"/>
@@ -2099,16 +2110,16 @@
       <c r="A549" s="5"/>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A550" s="6"/>
+      <c r="A550" s="5"/>
     </row>
     <row r="551" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A551" s="5"/>
+      <c r="A551" s="6"/>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A552" s="5"/>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A553" s="7"/>
+      <c r="A553" s="5"/>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A554" s="7"/>
@@ -2123,16 +2134,16 @@
       <c r="A557" s="7"/>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A558" s="5"/>
+      <c r="A558" s="7"/>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A559" s="6"/>
+      <c r="A559" s="5"/>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A560" s="6"/>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A561" s="5"/>
+      <c r="A561" s="6"/>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A562" s="5"/>
@@ -2144,7 +2155,7 @@
       <c r="A564" s="5"/>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A565" s="6"/>
+      <c r="A565" s="5"/>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A566" s="6"/>
@@ -2189,7 +2200,7 @@
       <c r="A579" s="6"/>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A580" s="5"/>
+      <c r="A580" s="6"/>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A581" s="5"/>
@@ -2198,7 +2209,7 @@
       <c r="A582" s="5"/>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A583" s="6"/>
+      <c r="A583" s="5"/>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A584" s="6"/>
@@ -2210,13 +2221,13 @@
       <c r="A586" s="6"/>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A587" s="5"/>
+      <c r="A587" s="6"/>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A588" s="6"/>
+      <c r="A588" s="5"/>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A589" s="5"/>
+      <c r="A589" s="6"/>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A590" s="5"/>
@@ -2228,7 +2239,7 @@
       <c r="A592" s="5"/>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A593" s="7"/>
+      <c r="A593" s="5"/>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A594" s="7"/>
@@ -2249,7 +2260,7 @@
       <c r="A599" s="7"/>
     </row>
     <row r="600" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A600" s="5"/>
+      <c r="A600" s="7"/>
     </row>
     <row r="601" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A601" s="5"/>
@@ -2261,7 +2272,7 @@
       <c r="A603" s="5"/>
     </row>
     <row r="604" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A604" s="7"/>
+      <c r="A604" s="5"/>
     </row>
     <row r="605" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A605" s="7"/>
@@ -2270,7 +2281,7 @@
       <c r="A606" s="7"/>
     </row>
     <row r="607" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A607" s="6"/>
+      <c r="A607" s="7"/>
     </row>
     <row r="608" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A608" s="6"/>
@@ -2291,13 +2302,13 @@
       <c r="A613" s="6"/>
     </row>
     <row r="614" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A614" s="5"/>
+      <c r="A614" s="6"/>
     </row>
     <row r="615" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A615" s="5"/>
     </row>
     <row r="616" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A616" s="6"/>
+      <c r="A616" s="5"/>
     </row>
     <row r="617" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A617" s="6"/>
@@ -2312,7 +2323,7 @@
       <c r="A620" s="6"/>
     </row>
     <row r="621" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A621" s="5"/>
+      <c r="A621" s="6"/>
     </row>
     <row r="622" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A622" s="5"/>
@@ -2327,7 +2338,7 @@
       <c r="A625" s="5"/>
     </row>
     <row r="626" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A626" s="6"/>
+      <c r="A626" s="5"/>
     </row>
     <row r="627" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A627" s="6"/>
@@ -2375,13 +2386,13 @@
       <c r="A641" s="6"/>
     </row>
     <row r="642" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A642" s="5"/>
+      <c r="A642" s="6"/>
     </row>
     <row r="643" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A643" s="6"/>
+      <c r="A643" s="5"/>
     </row>
     <row r="644" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A644" s="5"/>
+      <c r="A644" s="6"/>
     </row>
     <row r="645" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A645" s="5"/>
@@ -2408,10 +2419,10 @@
       <c r="A652" s="5"/>
     </row>
     <row r="653" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A653" s="6"/>
+      <c r="A653" s="5"/>
     </row>
     <row r="654" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A654" s="5"/>
+      <c r="A654" s="6"/>
     </row>
     <row r="655" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A655" s="5"/>
@@ -2429,10 +2440,10 @@
       <c r="A659" s="5"/>
     </row>
     <row r="660" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A660" s="6"/>
+      <c r="A660" s="5"/>
     </row>
     <row r="661" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A661" s="5"/>
+      <c r="A661" s="6"/>
     </row>
     <row r="662" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A662" s="5"/>
@@ -2444,7 +2455,7 @@
       <c r="A664" s="5"/>
     </row>
     <row r="665" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A665" s="6"/>
+      <c r="A665" s="5"/>
     </row>
     <row r="666" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A666" s="6"/>
@@ -2453,16 +2464,16 @@
       <c r="A667" s="6"/>
     </row>
     <row r="668" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A668" s="5"/>
+      <c r="A668" s="6"/>
     </row>
     <row r="669" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A669" s="5"/>
     </row>
     <row r="670" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A670" s="6"/>
+      <c r="A670" s="5"/>
     </row>
     <row r="671" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A671" s="5"/>
+      <c r="A671" s="6"/>
     </row>
     <row r="672" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A672" s="5"/>
@@ -2477,10 +2488,10 @@
       <c r="A675" s="5"/>
     </row>
     <row r="676" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A676" s="6"/>
+      <c r="A676" s="5"/>
     </row>
     <row r="677" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A677" s="5"/>
+      <c r="A677" s="6"/>
     </row>
     <row r="678" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A678" s="5"/>
@@ -2492,7 +2503,7 @@
       <c r="A680" s="5"/>
     </row>
     <row r="681" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A681" s="6"/>
+      <c r="A681" s="5"/>
     </row>
     <row r="682" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A682" s="6"/>
@@ -2507,13 +2518,13 @@
       <c r="A685" s="6"/>
     </row>
     <row r="686" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A686" s="5"/>
+      <c r="A686" s="6"/>
     </row>
     <row r="687" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A687" s="5"/>
     </row>
     <row r="688" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A688" s="6"/>
+      <c r="A688" s="5"/>
     </row>
     <row r="689" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A689" s="6"/>
@@ -2522,7 +2533,7 @@
       <c r="A690" s="6"/>
     </row>
     <row r="691" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A691" s="5"/>
+      <c r="A691" s="6"/>
     </row>
     <row r="692" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A692" s="5"/>
@@ -2531,10 +2542,10 @@
       <c r="A693" s="5"/>
     </row>
     <row r="694" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A694" s="6"/>
+      <c r="A694" s="5"/>
     </row>
     <row r="695" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A695" s="8"/>
+      <c r="A695" s="6"/>
     </row>
     <row r="696" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A696" s="8"/>
@@ -2579,7 +2590,7 @@
       <c r="A709" s="8"/>
     </row>
     <row r="710" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A710" s="9"/>
+      <c r="A710" s="8"/>
     </row>
     <row r="711" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A711" s="9"/>
@@ -2594,19 +2605,19 @@
       <c r="A714" s="9"/>
     </row>
     <row r="715" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A715" s="8"/>
+      <c r="A715" s="9"/>
     </row>
     <row r="716" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A716" s="8"/>
     </row>
     <row r="717" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A717" s="9"/>
+      <c r="A717" s="8"/>
     </row>
     <row r="718" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A718" s="9"/>
     </row>
     <row r="719" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A719" s="8"/>
+      <c r="A719" s="9"/>
     </row>
     <row r="720" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A720" s="8"/>
@@ -2621,7 +2632,7 @@
       <c r="A723" s="8"/>
     </row>
     <row r="724" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A724" s="9"/>
+      <c r="A724" s="8"/>
     </row>
     <row r="725" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A725" s="9"/>
@@ -2645,7 +2656,7 @@
       <c r="A731" s="9"/>
     </row>
     <row r="732" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A732" s="8"/>
+      <c r="A732" s="9"/>
     </row>
     <row r="733" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A733" s="8"/>
@@ -2669,10 +2680,10 @@
       <c r="A739" s="8"/>
     </row>
     <row r="740" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A740" s="9"/>
+      <c r="A740" s="8"/>
     </row>
     <row r="741" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A741" s="8"/>
+      <c r="A741" s="9"/>
     </row>
     <row r="742" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A742" s="8"/>
@@ -2705,7 +2716,7 @@
       <c r="A751" s="8"/>
     </row>
     <row r="752" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A752" s="9"/>
+      <c r="A752" s="8"/>
     </row>
     <row r="753" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A753" s="9"/>
@@ -2717,10 +2728,10 @@
       <c r="A755" s="9"/>
     </row>
     <row r="756" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A756" s="10"/>
+      <c r="A756" s="9"/>
     </row>
     <row r="757" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A757" s="8"/>
+      <c r="A757" s="10"/>
     </row>
     <row r="758" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A758" s="8"/>
@@ -2735,13 +2746,13 @@
       <c r="A761" s="8"/>
     </row>
     <row r="762" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A762" s="9"/>
+      <c r="A762" s="8"/>
     </row>
     <row r="763" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A763" s="8"/>
+      <c r="A763" s="9"/>
     </row>
     <row r="764" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A764" s="9"/>
+      <c r="A764" s="8"/>
     </row>
     <row r="765" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A765" s="9"/>
@@ -2750,13 +2761,13 @@
       <c r="A766" s="9"/>
     </row>
     <row r="767" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A767" s="8"/>
+      <c r="A767" s="9"/>
     </row>
     <row r="768" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A768" s="9"/>
+      <c r="A768" s="8"/>
     </row>
     <row r="769" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A769" s="8"/>
+      <c r="A769" s="9"/>
     </row>
     <row r="770" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A770" s="8"/>
@@ -2765,7 +2776,7 @@
       <c r="A771" s="8"/>
     </row>
     <row r="772" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A772" s="9"/>
+      <c r="A772" s="8"/>
     </row>
     <row r="773" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A773" s="9"/>
@@ -2780,7 +2791,7 @@
       <c r="A776" s="9"/>
     </row>
     <row r="777" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A777" s="8"/>
+      <c r="A777" s="9"/>
     </row>
     <row r="778" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A778" s="8"/>
@@ -2873,7 +2884,7 @@
       <c r="A807" s="8"/>
     </row>
     <row r="808" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A808" s="9"/>
+      <c r="A808" s="8"/>
     </row>
     <row r="809" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A809" s="9"/>
@@ -2882,7 +2893,7 @@
       <c r="A810" s="9"/>
     </row>
     <row r="811" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A811" s="8"/>
+      <c r="A811" s="9"/>
     </row>
     <row r="812" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A812" s="8"/>
@@ -2900,7 +2911,7 @@
       <c r="A816" s="8"/>
     </row>
     <row r="817" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A817" s="9"/>
+      <c r="A817" s="8"/>
     </row>
     <row r="818" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A818" s="9"/>
@@ -2924,7 +2935,7 @@
       <c r="A824" s="9"/>
     </row>
     <row r="825" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A825" s="8"/>
+      <c r="A825" s="9"/>
     </row>
     <row r="826" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A826" s="8"/>
@@ -2987,10 +2998,10 @@
       <c r="A845" s="8"/>
     </row>
     <row r="846" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A846" s="9"/>
+      <c r="A846" s="8"/>
     </row>
     <row r="847" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A847" s="8"/>
+      <c r="A847" s="9"/>
     </row>
     <row r="848" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A848" s="8"/>
@@ -3023,7 +3034,7 @@
       <c r="A857" s="8"/>
     </row>
     <row r="858" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A858" s="9"/>
+      <c r="A858" s="8"/>
     </row>
     <row r="859" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A859" s="9"/>
@@ -3047,10 +3058,10 @@
       <c r="A865" s="9"/>
     </row>
     <row r="866" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A866" s="8"/>
+      <c r="A866" s="9"/>
     </row>
     <row r="867" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A867" s="9"/>
+      <c r="A867" s="8"/>
     </row>
     <row r="868" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A868" s="9"/>
@@ -3062,13 +3073,13 @@
       <c r="A870" s="9"/>
     </row>
     <row r="871" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A871" s="8"/>
+      <c r="A871" s="9"/>
     </row>
     <row r="872" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A872" s="8"/>
     </row>
     <row r="873" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A873" s="9"/>
+      <c r="A873" s="8"/>
     </row>
     <row r="874" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A874" s="9"/>
@@ -3080,34 +3091,34 @@
       <c r="A876" s="9"/>
     </row>
     <row r="877" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A877" s="8"/>
+      <c r="A877" s="9"/>
     </row>
     <row r="878" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A878" s="9"/>
+      <c r="A878" s="8"/>
     </row>
     <row r="879" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A879" s="9"/>
     </row>
     <row r="880" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A880" s="8"/>
+      <c r="A880" s="9"/>
     </row>
     <row r="881" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A881" s="9"/>
+      <c r="A881" s="8"/>
     </row>
     <row r="882" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A882" s="9"/>
     </row>
     <row r="883" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A883" s="8"/>
+      <c r="A883" s="9"/>
     </row>
     <row r="884" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A884" s="9"/>
+      <c r="A884" s="8"/>
     </row>
     <row r="885" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A885" s="8"/>
+      <c r="A885" s="9"/>
     </row>
     <row r="886" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A886" s="9"/>
+      <c r="A886" s="8"/>
     </row>
     <row r="887" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A887" s="9"/>
@@ -3119,19 +3130,19 @@
       <c r="A889" s="9"/>
     </row>
     <row r="890" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A890" s="8"/>
+      <c r="A890" s="9"/>
     </row>
     <row r="891" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A891" s="9"/>
+      <c r="A891" s="8"/>
     </row>
     <row r="892" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A892" s="9"/>
     </row>
     <row r="893" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A893" s="8"/>
+      <c r="A893" s="9"/>
     </row>
     <row r="894" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A894" s="9"/>
+      <c r="A894" s="8"/>
     </row>
     <row r="895" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A895" s="9"/>
@@ -3149,7 +3160,7 @@
       <c r="A899" s="9"/>
     </row>
     <row r="900" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A900" s="8"/>
+      <c r="A900" s="9"/>
     </row>
     <row r="901" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A901" s="8"/>
@@ -3161,7 +3172,7 @@
       <c r="A903" s="8"/>
     </row>
     <row r="904" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A904" s="9"/>
+      <c r="A904" s="8"/>
     </row>
     <row r="905" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A905" s="9"/>
@@ -3170,7 +3181,7 @@
       <c r="A906" s="9"/>
     </row>
     <row r="907" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A907" s="8"/>
+      <c r="A907" s="9"/>
     </row>
     <row r="908" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A908" s="8"/>
@@ -3215,13 +3226,16 @@
       <c r="A921" s="8"/>
     </row>
     <row r="922" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A922" s="9"/>
+      <c r="A922" s="8"/>
     </row>
     <row r="923" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A923" s="9"/>
     </row>
     <row r="924" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A924" s="8"/>
+      <c r="A924" s="9"/>
+    </row>
+    <row r="925" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A925" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>